<commit_message>
feat: 新增 Rush 3 表單
</commit_message>
<xml_diff>
--- a/data/gaole.xlsx
+++ b/data/gaole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdvmedsNew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE82D37-CFEF-49C4-A64D-E25D9F4065D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC8A615-89CA-4546-9E9A-494248368818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="855" windowWidth="25125" windowHeight="11805" activeTab="5" xr2:uid="{80CAA787-1537-4523-969E-3FD1AC310A5E}"/>
+    <workbookView xWindow="2235" yWindow="3525" windowWidth="25125" windowHeight="11805" activeTab="6" xr2:uid="{80CAA787-1537-4523-969E-3FD1AC310A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend 1 彈" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Legend 4 彈" sheetId="1" r:id="rId4"/>
     <sheet name="Rush 1 彈" sheetId="2" r:id="rId5"/>
     <sheet name="Rush 2 彈" sheetId="7" r:id="rId6"/>
+    <sheet name="Rush 3 彈" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="468">
   <si>
     <t>1-利歐路</t>
   </si>
@@ -1455,12 +1456,381 @@
     <t>5-洛奇亞</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>2-頓甲</t>
+  </si>
+  <si>
+    <t>3-沙奈朵</t>
+  </si>
+  <si>
+    <t>4-克雷色利亞-R</t>
+  </si>
+  <si>
+    <t>4-皮卡丘-R</t>
+  </si>
+  <si>
+    <t>2-毒薔薇</t>
+  </si>
+  <si>
+    <t>1-咕咕</t>
+  </si>
+  <si>
+    <t>4-艾路雷朵</t>
+  </si>
+  <si>
+    <t>1-烏波</t>
+  </si>
+  <si>
+    <t>1-拉魯拉絲</t>
+  </si>
+  <si>
+    <t>2-貓頭夜鷹</t>
+  </si>
+  <si>
+    <t>5-基格爾德-R</t>
+  </si>
+  <si>
+    <t>2-奇魯莉安</t>
+  </si>
+  <si>
+    <t>1-滾滾蝙蝠</t>
+  </si>
+  <si>
+    <t>5-達克萊伊-R</t>
+  </si>
+  <si>
+    <r>
+      <t>4-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft JhengHei UI"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>艾路雷朵</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-艾路雷朵</t>
+  </si>
+  <si>
+    <t>3-沼王</t>
+  </si>
+  <si>
+    <t>2-沼王</t>
+  </si>
+  <si>
+    <t>2-心蝙蝠</t>
+  </si>
+  <si>
+    <t>3-貓頭夜鷹</t>
+  </si>
+  <si>
+    <t>4-土地雲</t>
+  </si>
+  <si>
+    <t>3-頓甲</t>
+  </si>
+  <si>
+    <t>1-小小象</t>
+  </si>
+  <si>
+    <t>4-龍捲雲</t>
+  </si>
+  <si>
+    <t>4-雷電雲</t>
+  </si>
+  <si>
+    <t>1-含羞苞</t>
+  </si>
+  <si>
+    <t>3-心蝙蝠</t>
+  </si>
+  <si>
+    <t>火稚雞</t>
+  </si>
+  <si>
+    <t>4-謝米-R</t>
+  </si>
+  <si>
+    <t>3-羅絲雷朵</t>
+  </si>
+  <si>
+    <t>4-沙奈朵</t>
+  </si>
+  <si>
+    <t>4-羅絲雷朵</t>
+  </si>
+  <si>
+    <t>2-烈咬陸鯊</t>
+  </si>
+  <si>
+    <t>5-謎擬Ｑ-R</t>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>雷吉奇卡斯</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>拉帝歐斯</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>腕力</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>固拉多</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>4-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>皮卡丘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-R</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>電束木</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>謎擬Ｑ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-R</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>伊裴爾塔爾</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>烈空坐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>虛無伊德</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>拉帝亞斯</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>蓋歐卡</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>哲爾尼亞斯</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1524,6 +1894,21 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei UI"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8637,8 +9022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4761F32F-7B25-4D63-BBA5-F321DCBFDB3C}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -9976,4 +10361,1349 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1A66B7-518A-41CD-AC3C-52F297779BF3}">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="8" width="14.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="4">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(File) feat: 新增 Rush 3 表單
</commit_message>
<xml_diff>
--- a/data/gaole.xlsx
+++ b/data/gaole.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdvmedsNew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC8A615-89CA-4546-9E9A-494248368818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597E7EE9-0DDD-4E31-883F-D768750D869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="3525" windowWidth="25125" windowHeight="11805" activeTab="6" xr2:uid="{80CAA787-1537-4523-969E-3FD1AC310A5E}"/>
+    <workbookView xWindow="4950" yWindow="4020" windowWidth="25125" windowHeight="11805" xr2:uid="{80CAA787-1537-4523-969E-3FD1AC310A5E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Legend 1 彈" sheetId="5" r:id="rId1"/>
-    <sheet name="Legend 2 彈" sheetId="4" r:id="rId2"/>
-    <sheet name="Legend 3 彈" sheetId="3" r:id="rId3"/>
-    <sheet name="Legend 4 彈" sheetId="1" r:id="rId4"/>
-    <sheet name="Rush 1 彈" sheetId="2" r:id="rId5"/>
-    <sheet name="Rush 2 彈" sheetId="7" r:id="rId6"/>
-    <sheet name="Rush 3 彈" sheetId="8" r:id="rId7"/>
+    <sheet name="Legend 2 彈" sheetId="4" r:id="rId1"/>
+    <sheet name="Legend 3 彈" sheetId="3" r:id="rId2"/>
+    <sheet name="Legend 4 彈" sheetId="1" r:id="rId3"/>
+    <sheet name="Rush 1 彈" sheetId="2" r:id="rId4"/>
+    <sheet name="Rush 2 彈" sheetId="7" r:id="rId5"/>
+    <sheet name="Rush 3 彈" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="402">
   <si>
     <t>1-利歐路</t>
   </si>
@@ -961,208 +960,10 @@
     <t>5-爆肌蚊</t>
   </si>
   <si>
-    <t>1-菊草葉</t>
-  </si>
-  <si>
-    <t>3-大竺葵</t>
-  </si>
-  <si>
-    <t>1-獨角犀牛</t>
-  </si>
-  <si>
-    <t>1-伊布</t>
-  </si>
-  <si>
-    <t>1-瑪瑙水母</t>
-  </si>
-  <si>
-    <t>1-火球鼠</t>
-  </si>
-  <si>
-    <t>3-樹才怪</t>
-  </si>
-  <si>
-    <t>2-樹才怪</t>
-  </si>
-  <si>
-    <t>2-火恐龍</t>
-  </si>
-  <si>
-    <t>4-雷伊布</t>
-  </si>
-  <si>
-    <t>2-月桂葉</t>
-  </si>
-  <si>
-    <t>3-火伊布</t>
-  </si>
-  <si>
-    <t>3-卡比獸</t>
-  </si>
-  <si>
-    <t>1-小火龍</t>
-  </si>
-  <si>
-    <t>3-超甲狂犀</t>
-  </si>
-  <si>
-    <t>1-傑尼龜</t>
-  </si>
-  <si>
-    <t>2-妙蛙草</t>
-  </si>
-  <si>
-    <t>2-火岩鼠</t>
-  </si>
-  <si>
-    <t>2-伊布</t>
-  </si>
-  <si>
-    <t>4-水箭龜</t>
-  </si>
-  <si>
-    <t>2-甲殼龍</t>
-  </si>
-  <si>
-    <t>1-小鋸鱷</t>
-  </si>
-  <si>
-    <t>4-皮卡丘</t>
-  </si>
-  <si>
-    <t>2-皮卡丘</t>
-  </si>
-  <si>
-    <t>4-大力鱷</t>
-  </si>
-  <si>
-    <t>2-鑽角犀獸</t>
-  </si>
-  <si>
-    <t>3-水箭龜</t>
-  </si>
-  <si>
-    <t>3-妙蛙花</t>
-  </si>
-  <si>
-    <t>5-超夢X</t>
-  </si>
-  <si>
-    <t>5-電束木</t>
-  </si>
-  <si>
-    <t>1-盆才怪</t>
-  </si>
-  <si>
-    <t>4-席多藍恩</t>
-  </si>
-  <si>
-    <t>1-妙蛙種子</t>
-  </si>
-  <si>
-    <t>4-暴飛龍</t>
-  </si>
-  <si>
-    <t>5-急涷鳥</t>
-  </si>
-  <si>
-    <t>2-藍鱷</t>
-  </si>
-  <si>
-    <t>5-火焰鳥</t>
-  </si>
-  <si>
-    <t>2-毒刺水母</t>
-  </si>
-  <si>
-    <t>1-寶貝龍</t>
-  </si>
-  <si>
-    <t>4-水伊布</t>
-  </si>
-  <si>
-    <t>3-雷伊布</t>
-  </si>
-  <si>
-    <t>4-噴火龍X</t>
-  </si>
-  <si>
-    <t>4-噴火龍Y</t>
-  </si>
-  <si>
-    <t>5-捷克羅姆</t>
-  </si>
-  <si>
-    <t>3-暴飛龍</t>
-  </si>
-  <si>
-    <t>4-美洛耶塔-綠</t>
-  </si>
-  <si>
-    <t>2-卡咪龜</t>
-  </si>
-  <si>
-    <t>3-大力鱷</t>
-  </si>
-  <si>
-    <t>4-瑪納霏</t>
-  </si>
-  <si>
-    <t>4-火爆獸</t>
-  </si>
-  <si>
-    <t>5-超夢Y</t>
-  </si>
-  <si>
-    <t>4-妙蛙花</t>
-  </si>
-  <si>
-    <t>3-火爆獸</t>
-  </si>
-  <si>
-    <t>3-水伊布</t>
-  </si>
-  <si>
-    <t>4-美洛耶塔-橙</t>
-  </si>
-  <si>
-    <t>3-噴火龍</t>
-  </si>
-  <si>
-    <t>4-蓋諾賽克特</t>
-  </si>
-  <si>
-    <t>3-毒刺水母</t>
-  </si>
-  <si>
     <t>4-巨鉗螳螂</t>
   </si>
   <si>
     <t>3-飛天螳螂</t>
-  </si>
-  <si>
-    <t>4-火伊布</t>
-  </si>
-  <si>
-    <t>5-閃電鳥</t>
-  </si>
-  <si>
-    <t>4-超甲狂犀</t>
-  </si>
-  <si>
-    <t>5-夢幻</t>
-  </si>
-  <si>
-    <t>4-克雷色利亞</t>
-  </si>
-  <si>
-    <t>5-虛吾伊德</t>
-  </si>
-  <si>
-    <t>5-萊希拉姆</t>
-  </si>
-  <si>
-    <t>4-大竺葵</t>
   </si>
   <si>
     <t>2-夢歌仙人掌</t>
@@ -1830,7 +1631,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1892,12 +1693,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Microsoft JhengHei UI"/>
       <family val="1"/>
       <charset val="136"/>
@@ -1952,7 +1747,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1975,9 +1770,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2293,1355 +2085,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734FFC75-5B4A-4FC5-A507-418BE18DE183}">
-  <dimension ref="A1:H51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="8" width="14.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="4">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4">
-        <v>6</v>
-      </c>
-      <c r="G1" s="4">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" thickBot="1">
-      <c r="A2" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" thickBot="1">
-      <c r="A3" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" thickBot="1">
-      <c r="A4" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" thickBot="1">
-      <c r="A5" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" thickBot="1">
-      <c r="A6" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" thickBot="1">
-      <c r="A7" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" thickBot="1">
-      <c r="A8" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" thickBot="1">
-      <c r="A9" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" thickBot="1">
-      <c r="A10" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" thickBot="1">
-      <c r="A11" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" thickBot="1">
-      <c r="A12" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" thickBot="1">
-      <c r="A13" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="18" thickBot="1">
-      <c r="A14" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18" thickBot="1">
-      <c r="A15" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="18" thickBot="1">
-      <c r="A16" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="18" thickBot="1">
-      <c r="A17" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18" thickBot="1">
-      <c r="A18" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18" thickBot="1">
-      <c r="A19" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="18" thickBot="1">
-      <c r="A20" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" thickBot="1">
-      <c r="A21" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18" thickBot="1">
-      <c r="A22" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="18" thickBot="1">
-      <c r="A23" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="18" thickBot="1">
-      <c r="A24" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="18" thickBot="1">
-      <c r="A25" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="18" thickBot="1">
-      <c r="A26" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="18" thickBot="1">
-      <c r="A27" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18" thickBot="1">
-      <c r="A28" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="18" thickBot="1">
-      <c r="A29" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="18" thickBot="1">
-      <c r="A30" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="18" thickBot="1">
-      <c r="A31" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="18" thickBot="1">
-      <c r="A32" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="18" thickBot="1">
-      <c r="A33" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="18" thickBot="1">
-      <c r="A34" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="18" thickBot="1">
-      <c r="A35" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="18" thickBot="1">
-      <c r="A36" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="18" thickBot="1">
-      <c r="A37" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="18" thickBot="1">
-      <c r="A38" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="18" thickBot="1">
-      <c r="A39" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="18" thickBot="1">
-      <c r="A40" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="18" thickBot="1">
-      <c r="A41" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="18" thickBot="1">
-      <c r="A42" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="18" thickBot="1">
-      <c r="A43" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="18" thickBot="1">
-      <c r="A44" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="18" thickBot="1">
-      <c r="A45" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="18" thickBot="1">
-      <c r="A46" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="18" thickBot="1">
-      <c r="A47" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="18" thickBot="1">
-      <c r="A48" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="18" thickBot="1">
-      <c r="A49" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="18" thickBot="1">
-      <c r="A50" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="18" thickBot="1">
-      <c r="A51" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DA9355-9932-43D6-9854-E2BFB3D62CFE}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -4982,7 +3429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9757F238-F30D-4581-A579-2F4EC684FD3E}">
   <dimension ref="A1:H51"/>
   <sheetViews>
@@ -6327,7 +4774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4415D778-A234-49F7-84D1-6E8D39E2E57E}">
   <dimension ref="A1:H51"/>
   <sheetViews>
@@ -7673,7 +6120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339D5A71-502A-4EA9-A0AB-378AD69CB425}">
   <dimension ref="A1:H51"/>
   <sheetViews>
@@ -9018,7 +7465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4761F32F-7B25-4D63-BBA5-F321DCBFDB3C}">
   <dimension ref="A1:H51"/>
   <sheetViews>
@@ -9059,701 +7506,701 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>384</v>
+        <v>318</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>390</v>
+        <v>324</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>406</v>
+        <v>340</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>405</v>
+        <v>339</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>410</v>
+        <v>344</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>395</v>
+        <v>329</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>390</v>
+        <v>324</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>399</v>
+        <v>333</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>390</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>416</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>417</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>398</v>
+        <v>332</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>378</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>352</v>
+        <v>286</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>400</v>
+        <v>334</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>406</v>
+        <v>340</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>364</v>
+        <v>298</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>352</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>413</v>
+        <v>347</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>398</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>355</v>
+        <v>289</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>369</v>
+        <v>303</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>395</v>
+        <v>329</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>389</v>
+        <v>323</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>399</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>356</v>
+        <v>290</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>373</v>
+        <v>307</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>393</v>
+        <v>327</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>400</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>411</v>
+        <v>345</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>373</v>
+        <v>307</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>404</v>
+        <v>338</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>418</v>
+        <v>352</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>409</v>
+        <v>343</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>411</v>
+        <v>345</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>107</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>373</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>393</v>
+        <v>327</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>389</v>
+        <v>323</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>410</v>
+        <v>344</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>402</v>
+        <v>336</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>386</v>
+        <v>320</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>384</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>411</v>
+        <v>345</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>395</v>
+        <v>329</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>401</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>364</v>
+        <v>298</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>356</v>
+        <v>290</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>367</v>
+        <v>301</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>410</v>
+        <v>344</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>378</v>
+        <v>312</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
-        <v>356</v>
+        <v>290</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>409</v>
+        <v>343</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>415</v>
+        <v>349</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>356</v>
+        <v>290</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>386</v>
+        <v>320</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>411</v>
+        <v>345</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>352</v>
+        <v>286</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>364</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>410</v>
+        <v>344</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>400</v>
+        <v>334</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>396</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>404</v>
+        <v>338</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>399</v>
+        <v>333</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>408</v>
+        <v>342</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
-        <v>367</v>
+        <v>301</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>414</v>
+        <v>348</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>405</v>
+        <v>339</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>404</v>
+        <v>338</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>369</v>
+        <v>303</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>385</v>
+        <v>319</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>376</v>
+        <v>310</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>107</v>
@@ -9761,600 +8208,600 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>413</v>
+        <v>347</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>367</v>
+        <v>301</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
-        <v>371</v>
+        <v>305</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>382</v>
+        <v>316</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>396</v>
+        <v>330</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>350</v>
+        <v>284</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>398</v>
+        <v>332</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>382</v>
+        <v>316</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>419</v>
+        <v>353</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>388</v>
+        <v>322</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>407</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
-        <v>373</v>
+        <v>307</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>378</v>
+        <v>312</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>350</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>405</v>
+        <v>339</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>406</v>
+        <v>340</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>363</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>415</v>
+        <v>349</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>350</v>
+        <v>284</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>384</v>
+        <v>318</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
-        <v>378</v>
+        <v>312</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>406</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>400</v>
+        <v>334</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>420</v>
+        <v>354</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>402</v>
+        <v>336</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>399</v>
+        <v>333</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>372</v>
+        <v>306</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>398</v>
+        <v>332</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>393</v>
+        <v>327</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>371</v>
+        <v>305</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>352</v>
+        <v>286</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>107</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>405</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="4" t="s">
-        <v>380</v>
+        <v>314</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>386</v>
+        <v>320</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>382</v>
+        <v>316</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>402</v>
+        <v>336</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>397</v>
+        <v>331</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>371</v>
+        <v>305</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>367</v>
+        <v>301</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
-        <v>382</v>
+        <v>316</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>412</v>
+        <v>346</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>396</v>
+        <v>330</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>413</v>
+        <v>347</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>413</v>
+        <v>347</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>404</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
-        <v>384</v>
+        <v>318</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>385</v>
+        <v>319</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>371</v>
+        <v>305</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>409</v>
+        <v>343</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>380</v>
+        <v>314</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>361</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>385</v>
+        <v>319</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>409</v>
+        <v>343</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>365</v>
+        <v>299</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>369</v>
+        <v>303</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>366</v>
+        <v>300</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>385</v>
+        <v>319</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>403</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>386</v>
+        <v>320</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>388</v>
+        <v>322</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>358</v>
+        <v>292</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>402</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>374</v>
+        <v>308</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>395</v>
+        <v>329</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>396</v>
+        <v>330</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>388</v>
+        <v>322</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>353</v>
+        <v>287</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>388</v>
+        <v>322</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>393</v>
+        <v>327</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>392</v>
+        <v>326</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
-        <v>389</v>
+        <v>323</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>359</v>
+        <v>293</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>364</v>
+        <v>298</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>390</v>
+        <v>324</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>369</v>
+        <v>303</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>391</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -10363,12 +8810,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1A66B7-518A-41CD-AC3C-52F297779BF3}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -10407,7 +8854,7 @@
         <v>226</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>179</v>
@@ -10419,13 +8866,13 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>422</v>
+        <v>356</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>424</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -10433,7 +8880,7 @@
         <v>226</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>425</v>
+        <v>359</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>223</v>
@@ -10445,7 +8892,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>18</v>
@@ -10456,7 +8903,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>455</v>
+        <v>389</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>239</v>
@@ -10477,18 +8924,18 @@
         <v>226</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>427</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>250</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>6</v>
@@ -10497,7 +8944,7 @@
         <v>223</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>226</v>
@@ -10508,22 +8955,22 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>223</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>431</v>
+        <v>365</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>456</v>
+        <v>390</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>184</v>
@@ -10534,19 +8981,19 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>457</v>
+        <v>391</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>422</v>
+        <v>356</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>239</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>168</v>
@@ -10563,22 +9010,22 @@
         <v>164</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>434</v>
+        <v>368</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>191</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>458</v>
+        <v>392</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>164</v>
@@ -10586,51 +9033,51 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
-        <v>435</v>
+        <v>369</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>248</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>436</v>
+        <v>370</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>437</v>
+        <v>371</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>459</v>
+        <v>393</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>158</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>424</v>
+        <v>358</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>6</v>
@@ -10638,7 +9085,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>440</v>
+        <v>374</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>154</v>
@@ -10647,39 +9094,39 @@
         <v>191</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>441</v>
+        <v>375</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>442</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>202</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>460</v>
+        <v>394</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>461</v>
+        <v>395</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>191</v>
@@ -10696,7 +9143,7 @@
         <v>154</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>239</v>
@@ -10708,67 +9155,67 @@
         <v>239</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>444</v>
+        <v>378</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>440</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>193</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>238</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>437</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>424</v>
+        <v>358</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>431</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>442</v>
+        <v>376</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>165</v>
@@ -10777,16 +9224,16 @@
         <v>168</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>248</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>436</v>
+        <v>370</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>248</v>
@@ -10794,28 +9241,28 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>444</v>
+        <v>378</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>436</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -10832,13 +9279,13 @@
         <v>236</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>58</v>
@@ -10846,51 +9293,51 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>437</v>
+        <v>371</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>442</v>
+        <v>376</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>422</v>
+        <v>356</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>168</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>448</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>226</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>195</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>239</v>
@@ -10904,10 +9351,10 @@
         <v>242</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>449</v>
+        <v>383</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>236</v>
@@ -10924,7 +9371,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>163</v>
@@ -10939,39 +9386,39 @@
         <v>191</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>427</v>
+        <v>361</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>164</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>436</v>
+        <v>370</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>226</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>449</v>
+        <v>383</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -10979,13 +9426,13 @@
         <v>223</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>451</v>
+        <v>385</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>206</v>
@@ -10994,7 +9441,7 @@
         <v>238</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>451</v>
+        <v>385</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>154</v>
@@ -11005,13 +9452,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>462</v>
+        <v>396</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>164</v>
@@ -11020,10 +9467,10 @@
         <v>6</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -11031,45 +9478,45 @@
         <v>158</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>191</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>447</v>
+        <v>381</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>463</v>
+        <v>397</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>154</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>195</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>439</v>
+        <v>373</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>239</v>
@@ -11089,7 +9536,7 @@
         <v>191</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>239</v>
@@ -11098,7 +9545,7 @@
         <v>154</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>168</v>
@@ -11112,22 +9559,22 @@
         <v>193</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>168</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -11138,19 +9585,19 @@
         <v>238</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>193</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>436</v>
+        <v>370</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>195</v>
@@ -11164,13 +9611,13 @@
         <v>158</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>441</v>
+        <v>375</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>440</v>
+        <v>374</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>163</v>
@@ -11187,22 +9634,22 @@
         <v>239</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>422</v>
+        <v>356</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>165</v>
@@ -11210,28 +9657,28 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>425</v>
+        <v>359</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>444</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -11248,10 +9695,10 @@
         <v>158</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>464</v>
+        <v>398</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>250</v>
@@ -11262,45 +9709,45 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>453</v>
+        <v>387</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>440</v>
+        <v>374</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>164</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>248</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>451</v>
+        <v>385</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
-        <v>451</v>
+        <v>385</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>453</v>
+        <v>387</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>422</v>
+        <v>356</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>441</v>
+        <v>375</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>18</v>
@@ -11317,16 +9764,16 @@
         <v>238</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>154</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>442</v>
+        <v>376</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>236</v>
@@ -11335,24 +9782,24 @@
         <v>195</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
-        <v>434</v>
+        <v>368</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>191</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>465</v>
+        <v>399</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>433</v>
+        <v>367</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>466</v>
+        <v>400</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>10</v>
@@ -11361,7 +9808,7 @@
         <v>164</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -11381,10 +9828,10 @@
         <v>163</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>425</v>
+        <v>359</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>154</v>
@@ -11395,10 +9842,10 @@
         <v>10</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>223</v>
@@ -11407,10 +9854,10 @@
         <v>164</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>168</v>
@@ -11436,15 +9883,15 @@
         <v>164</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
-        <v>450</v>
+        <v>384</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>193</v>
@@ -11453,19 +9900,19 @@
         <v>163</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>158</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -11473,13 +9920,13 @@
         <v>206</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>239</v>
@@ -11496,19 +9943,19 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>226</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>226</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>437</v>
+        <v>371</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>206</v>
@@ -11522,16 +9969,16 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>441</v>
+        <v>375</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>444</v>
+        <v>378</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>467</v>
+        <v>401</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>202</v>
@@ -11551,25 +9998,25 @@
         <v>191</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>250</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -11577,16 +10024,16 @@
         <v>154</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>191</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>165</v>
@@ -11595,21 +10042,21 @@
         <v>58</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>446</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>452</v>
+        <v>386</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>449</v>
+        <v>383</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>223</v>
@@ -11629,22 +10076,22 @@
         <v>179</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>442</v>
+        <v>376</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>427</v>
+        <v>361</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>158</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>445</v>
+        <v>379</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>454</v>
+        <v>388</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>206</v>
@@ -11652,28 +10099,28 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>430</v>
+        <v>364</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>239</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>453</v>
+        <v>387</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>421</v>
+        <v>355</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>438</v>
+        <v>372</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>426</v>
+        <v>360</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -11681,22 +10128,22 @@
         <v>193</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>449</v>
+        <v>383</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>443</v>
+        <v>377</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>165</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>425</v>
+        <v>359</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>250</v>

</xml_diff>